<commit_message>
Update function create district
</commit_message>
<xml_diff>
--- a/Template_Import/ImportCity_v1.xlsx
+++ b/Template_Import/ImportCity_v1.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development_Project\Dev_ManagerMusic\Source\ManagerMusic\Template_Import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\v_3\ManagerMusic\Template_Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91164117-5235-4FCF-9E9C-E093BC71954E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3972" yWindow="2448" windowWidth="23088" windowHeight="11292"/>
+    <workbookView xWindow="12705" yWindow="0" windowWidth="11955" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="104">
   <si>
     <t>STT</t>
   </si>
@@ -323,12 +324,36 @@
   </si>
   <si>
     <t>Mã Vị Trí</t>
+  </si>
+  <si>
+    <t>Tỉnh Thừa Thiên Huế</t>
+  </si>
+  <si>
+    <t>TTH</t>
+  </si>
+  <si>
+    <t>Tỉnh Đồng Nai</t>
+  </si>
+  <si>
+    <t>ĐN</t>
+  </si>
+  <si>
+    <t>Tỉnh Bà Rịa-Vũng Tàu</t>
+  </si>
+  <si>
+    <t>BR-VT</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>Thành Phố Cần Thơ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -732,28 +757,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="8.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="10" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="10" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -772,13 +797,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D3" s="9">
-        <v>263</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -786,13 +811,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D4" s="9">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -800,13 +825,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D5" s="9">
-        <v>276</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -814,13 +839,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D6" s="9">
-        <v>256</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -828,13 +853,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="D7" s="9">
-        <v>271</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -842,13 +867,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="D8" s="9">
-        <v>252</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -856,601 +881,643 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D9" s="9">
-        <v>290</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D10" s="9">
-        <v>206</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D11" s="9">
-        <v>262</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D12" s="9">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D13" s="9">
-        <v>269</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="D14" s="9">
-        <v>219</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D15" s="9">
-        <v>226</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D16" s="9">
-        <v>239</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D17" s="9">
-        <v>220</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D18" s="9">
-        <v>225</v>
+        <v>293</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D19" s="9">
-        <v>293</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D20" s="9">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="D21" s="9">
-        <v>221</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="D22" s="9">
-        <v>258</v>
+        <v>297</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D23" s="9">
-        <v>297</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D24" s="9">
-        <v>260</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D25" s="9">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D26" s="9">
-        <v>205</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D27" s="9">
-        <v>214</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
+        <v>26</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>2</v>
-      </c>
       <c r="C28" s="9" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="D28" s="9">
-        <v>263</v>
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
+        <v>27</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="C29" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D29" s="9">
-        <v>272</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
+        <v>28</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="C30" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D30" s="9">
-        <v>228</v>
+        <v>238</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
+        <v>29</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="C31" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D31" s="9">
-        <v>238</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
+        <v>30</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="C32" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D32" s="9">
-        <v>229</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
+        <v>31</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="C33" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D33" s="9">
-        <v>259</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
+        <v>32</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="C34" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D34" s="9">
-        <v>210</v>
+        <v>257</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
+        <v>33</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="C35" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D35" s="9">
-        <v>257</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
+        <v>34</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="C36" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D36" s="9">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
+        <v>35</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>80</v>
       </c>
       <c r="D37" s="9">
-        <v>235</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
+        <v>36</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>80</v>
       </c>
       <c r="D38" s="9">
-        <v>255</v>
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
+        <v>37</v>
+      </c>
+      <c r="B39" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="8" t="s">
-        <v>37</v>
-      </c>
       <c r="C39" s="9" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D39" s="9">
-        <v>203</v>
+        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
+        <v>38</v>
+      </c>
+      <c r="B40" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="C40" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D40" s="9">
-        <v>233</v>
+        <v>299</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
+        <v>39</v>
+      </c>
+      <c r="B41" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="C41" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D41" s="9">
-        <v>299</v>
+        <v>212</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
+        <v>40</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="C42" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D42" s="9">
-        <v>212</v>
+        <v>276</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
+        <v>41</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>87</v>
       </c>
       <c r="D43" s="9">
-        <v>276</v>
+        <v>208</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
+        <v>42</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="C44" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D44" s="9">
-        <v>208</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
+        <v>43</v>
+      </c>
+      <c r="B45" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>43</v>
-      </c>
       <c r="C45" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D45" s="9">
-        <v>237</v>
+        <v>273</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
+        <v>44</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="C46" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D46" s="9">
-        <v>273</v>
+        <v>294</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
+        <v>45</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>45</v>
-      </c>
       <c r="C47" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D47" s="9">
-        <v>294</v>
+        <v>207</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
+        <v>46</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="C48" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D48" s="9">
-        <v>207</v>
+        <v>270</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
+        <v>47</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="C49" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D49" s="9">
-        <v>270</v>
+        <v>211</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
+        <v>48</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="C50" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D50" s="9">
-        <v>211</v>
+        <v>216</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
+        <v>49</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" s="9">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
         <v>50</v>
       </c>
-      <c r="B51" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D51" s="9">
-        <v>216</v>
+      <c r="B52" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D52" s="9">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
+        <v>51</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D53" s="9">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
+        <v>52</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D54" s="9">
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>